<commit_message>
reconig TP5, including accidently removing the spring check and last subset of snyder(without name) lines, also reordered columns to match other TP ones
</commit_message>
<xml_diff>
--- a/data/Winter_DH/TP5/DHtp5_all_ter_edit.xlsx
+++ b/data/Winter_DH/TP5/DHtp5_all_ter_edit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Google Drive\Grad School_\Field 2020\Winter_Grains\Germination_consolidation\TP5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\git\BarleyGermination-KK\data\Winter_DH\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBDDD47-2B6C-439F-AD39-18DA4EF70B83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4FF379-2934-4DA7-A237-B8DB25D35868}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{02223FC2-60EF-4F6C-88D9-3658E3ABE109}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4476" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4496" uniqueCount="495">
   <si>
     <t>Entry</t>
   </si>
@@ -1501,6 +1501,15 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>SRBBBdormSNLine</t>
+  </si>
+  <si>
+    <t>SNBBBdormSNLine</t>
+  </si>
+  <si>
+    <t>BS614-35</t>
   </si>
 </sst>
 </file>
@@ -1869,8 +1878,8 @@
   <dimension ref="A1:R982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A850" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A865" sqref="A865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39563,6 +39572,9 @@
       </c>
     </row>
     <row r="853" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A853" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="B853" s="2" t="s">
         <v>30</v>
       </c>
@@ -39595,6 +39607,9 @@
       </c>
     </row>
     <row r="854" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A854" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="B854" s="2" t="s">
         <v>29</v>
       </c>
@@ -39627,6 +39642,9 @@
       </c>
     </row>
     <row r="855" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A855" s="1" t="s">
+        <v>494</v>
+      </c>
       <c r="B855" s="2" t="s">
         <v>28</v>
       </c>
@@ -39659,6 +39677,9 @@
       </c>
     </row>
     <row r="856" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A856" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="B856" s="2" t="s">
         <v>27</v>
       </c>
@@ -39691,6 +39712,9 @@
       </c>
     </row>
     <row r="857" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A857" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="B857" s="2" t="s">
         <v>26</v>
       </c>
@@ -39723,6 +39747,9 @@
       </c>
     </row>
     <row r="858" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A858" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B858" s="2" t="s">
         <v>25</v>
       </c>
@@ -39755,6 +39782,9 @@
       </c>
     </row>
     <row r="859" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A859" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B859" s="2" t="s">
         <v>24</v>
       </c>
@@ -39787,6 +39817,9 @@
       </c>
     </row>
     <row r="860" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A860" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B860" s="2" t="s">
         <v>23</v>
       </c>
@@ -39819,6 +39852,9 @@
       </c>
     </row>
     <row r="861" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A861" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B861" s="2" t="s">
         <v>22</v>
       </c>
@@ -39851,6 +39887,9 @@
       </c>
     </row>
     <row r="862" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A862" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="B862" s="2" t="s">
         <v>19</v>
       </c>
@@ -39883,6 +39922,9 @@
       </c>
     </row>
     <row r="863" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A863" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="B863" s="2" t="s">
         <v>18</v>
       </c>
@@ -39915,6 +39957,9 @@
       </c>
     </row>
     <row r="864" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A864" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="B864" s="2" t="s">
         <v>17</v>
       </c>
@@ -39946,7 +39991,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="865" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="865" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A865" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="B865" s="2" t="s">
         <v>16</v>
       </c>
@@ -39978,7 +40026,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="866" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="866" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A866" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="B866" s="2" t="s">
         <v>15</v>
       </c>
@@ -40010,7 +40061,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="867" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="867" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A867" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="B867" s="2" t="s">
         <v>12</v>
       </c>
@@ -40042,7 +40096,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="868" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="868" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A868" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="B868" s="2" t="s">
         <v>484</v>
       </c>
@@ -40089,7 +40146,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="869" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="869" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A869" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="B869" s="2" t="s">
         <v>483</v>
       </c>
@@ -40136,7 +40196,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="870" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="870" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A870" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="B870" s="2" t="s">
         <v>482</v>
       </c>
@@ -40183,7 +40246,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="871" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="871" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A871" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="B871" s="2" t="s">
         <v>481</v>
       </c>
@@ -40230,7 +40296,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="872" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="872" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A872" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="B872" s="2" t="s">
         <v>480</v>
       </c>

</xml_diff>